<commit_message>
First semi working code
Code works up to 54th inning and then starts to assign multiple people to benched.
</commit_message>
<xml_diff>
--- a/data/Baseball_Roster.xlsx
+++ b/data/Baseball_Roster.xlsx
@@ -1,23 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr showInkAnnotation="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paul\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paul\Documents\Code\random-team\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22000499-F499-499E-AE54-E4F588591FE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{857D4367-781A-45B6-89EF-FEFC737FF431}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6735" yWindow="2820" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Players" sheetId="1" r:id="rId1"/>
     <sheet name="Positions" sheetId="2" r:id="rId2"/>
-    <sheet name="Rules" sheetId="3" r:id="rId3"/>
+    <sheet name="Rules - Not working" sheetId="3" r:id="rId3"/>
+    <sheet name="Details" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
   <si>
     <t>Cole</t>
   </si>
@@ -125,6 +127,21 @@
   </si>
   <si>
     <t>In_Out</t>
+  </si>
+  <si>
+    <t>Rule_Word</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Min_Infield_Inning</t>
+  </si>
+  <si>
+    <t>Position_Restricted</t>
   </si>
 </sst>
 </file>
@@ -140,12 +157,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -160,8 +183,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -478,8 +502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D7EA05A-454D-164F-BD9B-2DC68160C030}">
   <dimension ref="A1:A12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,27 +514,27 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -520,27 +544,27 @@
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -554,7 +578,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A5" sqref="A5:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -571,82 +595,82 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>29</v>
       </c>
     </row>
@@ -657,10 +681,63 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03A837E7-C381-4FD9-ACA0-2E02562979D5}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="125.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5400D80-081F-41CA-BB91-3F87A1F2F98D}">
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -668,26 +745,18 @@
     <col min="1" max="1" width="125.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Corrected and working code
Added additional checks and validations for the total number of infield positions assigned. If the randomization doesn't work out, then run until it does. Will optimize the code later.
</commit_message>
<xml_diff>
--- a/data/Baseball_Roster.xlsx
+++ b/data/Baseball_Roster.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paul\Documents\Code\random-team\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{857D4367-781A-45B6-89EF-FEFC737FF431}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69E669C2-64DB-4FA4-A7E3-1F46FA14D384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Players" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <sheet name="Details" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="47">
   <si>
     <t>Cole</t>
   </si>
@@ -142,6 +141,39 @@
   </si>
   <si>
     <t>Position_Restricted</t>
+  </si>
+  <si>
+    <t>Main Inning 5: Player John is in position 1ST, INFIELD</t>
+  </si>
+  <si>
+    <t>Main Inning 5: Player Luke B is in position LC, OUTFIELD</t>
+  </si>
+  <si>
+    <t>Main Inning 5: Player Luke M is in position RF, OUTFIELD</t>
+  </si>
+  <si>
+    <t>Main Inning 5: Player Grayson is in position 3RD, INFIELD</t>
+  </si>
+  <si>
+    <t>Main Inning 5: Player Sean is in position RC, OUTFIELD</t>
+  </si>
+  <si>
+    <t>Main Inning 5: Player Graham is in position BENCHED, BENCHED</t>
+  </si>
+  <si>
+    <t>Main Inning 5: Player Ryan is in position BENCHED, BENCHED</t>
+  </si>
+  <si>
+    <t>Main Inning 5: Player Luca is in position 2ND, INFIELD</t>
+  </si>
+  <si>
+    <t>Main Inning 5: Player Cole is in position C, INFIELD</t>
+  </si>
+  <si>
+    <t>Main Inning 5: Player Colton is in position LF, OUTFIELD</t>
+  </si>
+  <si>
+    <t>Main Inning 5: Player Griffin is in position SS, INFIELD</t>
   </si>
 </sst>
 </file>
@@ -183,9 +215,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -503,7 +536,7 @@
   <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,10 +608,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFA98480-D0D6-4CE9-9FBA-338339932BF1}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:B5"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -586,92 +619,125 @@
     <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>16</v>
       </c>
       <c r="B1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="I1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="I2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="I3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="I4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="I5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="I6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="I7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="I8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="I9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="I10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="I11" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -683,7 +749,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03A837E7-C381-4FD9-ACA0-2E02562979D5}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
@@ -736,7 +802,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5400D80-081F-41CA-BB91-3F87A1F2F98D}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>

</xml_diff>